<commit_message>
Fix Diaza's second initial
</commit_message>
<xml_diff>
--- a/11-CollaborationList/Imperial.xlsx
+++ b/11-CollaborationList/Imperial.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11122"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10110"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kennethlong/Library/CloudStorage/Box-Box/CubMac-Box/KL-GIT/CCAP/02-LhARA/00-Collaboration-lists/11-CollaborationList/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://api.box.com/wopi/files/2050113224685/WOPIServiceId_TP_BOX_2/WOPIUserId_-/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96E5052D-56CD-784F-9B91-457CD138E2B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{96E5052D-56CD-784F-9B91-457CD138E2B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A403DB19-A7EB-3C48-BA6C-CDD64138C8F0}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{7B5F04B9-63DF-474E-BF2F-8D8D82A0D772}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="188">
   <si>
     <t>Title</t>
   </si>
@@ -581,6 +581,9 @@
   </si>
   <si>
     <t>Department of Computing, Imperial College London, Exhibition Road, London, SW7 2AZ, UK</t>
+  </si>
+  <si>
+    <t>D.O.</t>
   </si>
 </sst>
 </file>
@@ -1482,8 +1485,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81C3A07F-0925-B14D-9B78-C81CB9121297}">
   <dimension ref="A1:P28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="L21" sqref="L21:M21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2413,7 +2416,7 @@
         <v>168</v>
       </c>
       <c r="D26" t="s">
-        <v>55</v>
+        <v>187</v>
       </c>
       <c r="E26" s="1" t="s">
         <v>166</v>

</xml_diff>

<commit_message>
Add LMU, fix initials, fix email list
</commit_message>
<xml_diff>
--- a/11-CollaborationList/Imperial.xlsx
+++ b/11-CollaborationList/Imperial.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://api.box.com/wopi/files/2050113224685/WOPIServiceId_TP_BOX_2/WOPIUserId_-/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{96E5052D-56CD-784F-9B91-457CD138E2B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A403DB19-A7EB-3C48-BA6C-CDD64138C8F0}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{96E5052D-56CD-784F-9B91-457CD138E2B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{08CCA064-1F79-5747-A25F-1497DE82ED19}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{7B5F04B9-63DF-474E-BF2F-8D8D82A0D772}"/>
   </bookViews>
@@ -550,9 +550,6 @@
     <t>N. Zakhir</t>
   </si>
   <si>
-    <t>N,</t>
-  </si>
-  <si>
     <t>zaynabsadur@gmail.com</t>
   </si>
   <si>
@@ -584,6 +581,9 @@
   </si>
   <si>
     <t>D.O.</t>
+  </si>
+  <si>
+    <t>N.</t>
   </si>
 </sst>
 </file>
@@ -1486,7 +1486,7 @@
   <dimension ref="A1:P28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1672,7 +1672,7 @@
         <v>30</v>
       </c>
       <c r="H5" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="I5">
         <v>0</v>
@@ -1969,19 +1969,19 @@
         <v>16</v>
       </c>
       <c r="B14" t="s">
+        <v>178</v>
+      </c>
+      <c r="C14" t="s">
         <v>179</v>
       </c>
-      <c r="C14" t="s">
+      <c r="D14" t="s">
         <v>180</v>
       </c>
-      <c r="D14" t="s">
+      <c r="E14" t="s">
         <v>181</v>
       </c>
-      <c r="E14" t="s">
+      <c r="F14" t="s">
         <v>182</v>
-      </c>
-      <c r="F14" t="s">
-        <v>183</v>
       </c>
       <c r="G14" t="s">
         <v>64</v>
@@ -2142,7 +2142,7 @@
         <v>94</v>
       </c>
       <c r="F18" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="G18" t="s">
         <v>64</v>
@@ -2300,7 +2300,7 @@
         <v>134</v>
       </c>
       <c r="F22" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="G22" t="s">
         <v>64</v>
@@ -2332,7 +2332,7 @@
         <v>115</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="F23" t="s">
         <v>174</v>
@@ -2387,10 +2387,10 @@
         <v>173</v>
       </c>
       <c r="D25" t="s">
-        <v>176</v>
+        <v>187</v>
       </c>
       <c r="E25" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F25" t="s">
         <v>175</v>
@@ -2416,7 +2416,7 @@
         <v>168</v>
       </c>
       <c r="D26" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E26" s="1" t="s">
         <v>166</v>

</xml_diff>

<commit_message>
Final fixes to IMperial and santiago
</commit_message>
<xml_diff>
--- a/11-CollaborationList/Imperial.xlsx
+++ b/11-CollaborationList/Imperial.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10118"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://api.box.com/wopi/files/2050113224685/WOPIServiceId_TP_BOX_2/WOPIUserId_-/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{96E5052D-56CD-784F-9B91-457CD138E2B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{08CCA064-1F79-5747-A25F-1497DE82ED19}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="13_ncr:1_{96E5052D-56CD-784F-9B91-457CD138E2B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7878E71E-2A78-9D49-9A12-EA3B692F8344}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{7B5F04B9-63DF-474E-BF2F-8D8D82A0D772}"/>
   </bookViews>
@@ -535,18 +535,12 @@
     <t>Zaynab</t>
   </si>
   <si>
-    <t>Sadhur</t>
-  </si>
-  <si>
     <t>Nadirah</t>
   </si>
   <si>
     <t>Zakhir</t>
   </si>
   <si>
-    <t>Z. Sadhur</t>
-  </si>
-  <si>
     <t>N. Zakhir</t>
   </si>
   <si>
@@ -584,6 +578,12 @@
   </si>
   <si>
     <t>N.</t>
+  </si>
+  <si>
+    <t>Sadur</t>
+  </si>
+  <si>
+    <t>Z. Sadur</t>
   </si>
 </sst>
 </file>
@@ -1486,7 +1486,7 @@
   <dimension ref="A1:P28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1672,7 +1672,7 @@
         <v>30</v>
       </c>
       <c r="H5" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="I5">
         <v>0</v>
@@ -1969,19 +1969,19 @@
         <v>16</v>
       </c>
       <c r="B14" t="s">
+        <v>176</v>
+      </c>
+      <c r="C14" t="s">
+        <v>177</v>
+      </c>
+      <c r="D14" t="s">
         <v>178</v>
       </c>
-      <c r="C14" t="s">
+      <c r="E14" t="s">
         <v>179</v>
       </c>
-      <c r="D14" t="s">
+      <c r="F14" t="s">
         <v>180</v>
-      </c>
-      <c r="E14" t="s">
-        <v>181</v>
-      </c>
-      <c r="F14" t="s">
-        <v>182</v>
       </c>
       <c r="G14" t="s">
         <v>64</v>
@@ -2142,7 +2142,7 @@
         <v>94</v>
       </c>
       <c r="F18" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="G18" t="s">
         <v>64</v>
@@ -2300,7 +2300,7 @@
         <v>134</v>
       </c>
       <c r="F22" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="G22" t="s">
         <v>64</v>
@@ -2326,16 +2326,16 @@
         <v>170</v>
       </c>
       <c r="C23" t="s">
-        <v>171</v>
+        <v>186</v>
       </c>
       <c r="D23" t="s">
         <v>115</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="F23" t="s">
-        <v>174</v>
+        <v>187</v>
       </c>
       <c r="G23" t="s">
         <v>64</v>
@@ -2381,19 +2381,19 @@
         <v>141</v>
       </c>
       <c r="B25" t="s">
+        <v>171</v>
+      </c>
+      <c r="C25" t="s">
         <v>172</v>
       </c>
-      <c r="C25" t="s">
+      <c r="D25" t="s">
+        <v>185</v>
+      </c>
+      <c r="E25" t="s">
+        <v>175</v>
+      </c>
+      <c r="F25" t="s">
         <v>173</v>
-      </c>
-      <c r="D25" t="s">
-        <v>187</v>
-      </c>
-      <c r="E25" t="s">
-        <v>177</v>
-      </c>
-      <c r="F25" t="s">
-        <v>175</v>
       </c>
       <c r="G25" t="s">
         <v>64</v>
@@ -2416,7 +2416,7 @@
         <v>168</v>
       </c>
       <c r="D26" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="E26" s="1" t="s">
         <v>166</v>

</xml_diff>